<commit_message>
Deployed 3c77e215 with MkDocs version: 1.1.2
</commit_message>
<xml_diff>
--- a/doc/scallop-inf1.xlsx
+++ b/doc/scallop-inf1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhz22\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCB4660-8382-4AF8-A106-FFDC1019C9CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6828A4-0B76-4EB4-AA98-AB936EFB985E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -923,277 +923,277 @@
     <t>VEGF.A.tsv.gz</t>
   </si>
   <si>
-    <t>8f13fbc0633df170e4029ba52b879e88</t>
-  </si>
-  <si>
-    <t>c4833bb1ff6ec117bfea316147b2feba</t>
-  </si>
-  <si>
-    <t>8645e6bf9804153c14482dd3032aa4d3</t>
-  </si>
-  <si>
-    <t>7e0ff1c1ad7bcc54e7eb4d36f30897e2</t>
-  </si>
-  <si>
-    <t>32766bfbe563a94c6d6cd1a10641f571</t>
-  </si>
-  <si>
-    <t>56cfe4810785087e886cc5c90297cf28</t>
-  </si>
-  <si>
-    <t>566c3e9cc2d61d71f12c28b475118ed7</t>
-  </si>
-  <si>
-    <t>10ddbfaaea5e796885c04712aac299a5</t>
-  </si>
-  <si>
-    <t>e69945b3209b695c41d98bced7623722</t>
-  </si>
-  <si>
-    <t>b4e56f47eaf8a1c3259a7196fb62e1ea</t>
-  </si>
-  <si>
-    <t>c7efbe305bf961598335bbd461d3f98f</t>
-  </si>
-  <si>
-    <t>95e72be62706378850b621f05a660df3</t>
-  </si>
-  <si>
-    <t>c52019ffd5cb4ccb8f9c2d2ce4182930</t>
-  </si>
-  <si>
-    <t>986c7f7692a0dac4ac9d34486d0dbf65</t>
-  </si>
-  <si>
-    <t>5f86e559f8b41b6aebcc09f4f45dd940</t>
-  </si>
-  <si>
-    <t>6731bacdd0253c324281996132ab3a58</t>
-  </si>
-  <si>
-    <t>75b0aaa677004a189b09931b5ee7dd24</t>
-  </si>
-  <si>
-    <t>9fd3d2cd20cf47e0b14e5cff4d5da351</t>
-  </si>
-  <si>
-    <t>a2ce2406b7362c3be802ec614718d6ac</t>
-  </si>
-  <si>
-    <t>aa67b7aedcd901e52554573416b47dae</t>
-  </si>
-  <si>
-    <t>a8f08c7fe0ad7206df6deaaf8597b648</t>
-  </si>
-  <si>
-    <t>be58ef3f3454386c03f9e2caaa7f8acb</t>
-  </si>
-  <si>
-    <t>fc30729990735d4ccd12ce56b9451a12</t>
-  </si>
-  <si>
-    <t>5fec4179316390f615e8a39ebeb6422f</t>
-  </si>
-  <si>
-    <t>cbecd15fdbb8c175c949a83dfed36e0b</t>
-  </si>
-  <si>
-    <t>67b496d595ccd1f5be76e2553f113b44</t>
-  </si>
-  <si>
-    <t>67d95d25e508e1fd022846412ea1fb7a</t>
-  </si>
-  <si>
-    <t>8185fcd41d1a805d5704a770ab10d6c1</t>
-  </si>
-  <si>
-    <t>f3bf2b6e0fb08b9a1ad3c635620b97b3</t>
-  </si>
-  <si>
-    <t>fb0ae032a73cadb0336e6c2cb4bf55e6</t>
-  </si>
-  <si>
-    <t>1257a0dd4c2b939320a454cedd467463</t>
-  </si>
-  <si>
-    <t>896da3ab031ffd74879a2ba4138a0249</t>
-  </si>
-  <si>
-    <t>996afee5112a76a555c16e2635dcc3cb</t>
-  </si>
-  <si>
-    <t>3241d28b208cc0d27e2c9f428a517fd4</t>
-  </si>
-  <si>
-    <t>5f6ce870139604933d3a7440d2f93b7d</t>
-  </si>
-  <si>
-    <t>8eda8974221cc3f24d20e16e8099e4e7</t>
-  </si>
-  <si>
-    <t>1c06883153ac852b4fcc19b087c6014f</t>
-  </si>
-  <si>
-    <t>703b7650c67b94f9f2bd09a285b247eb</t>
-  </si>
-  <si>
-    <t>80fb9f9db4e5e7e46d51d2e0f3a69aaa</t>
-  </si>
-  <si>
-    <t>4e9e5d0fa15743b53247d9ccd3793d5b</t>
-  </si>
-  <si>
-    <t>83f7f61f69d2d835ac4ceb5f94401fcb</t>
-  </si>
-  <si>
-    <t>afa9dddf9ce26c64a9d27d55ecbd85b2</t>
-  </si>
-  <si>
-    <t>3f9146a6740920cfdfcd70c7b1f74f88</t>
-  </si>
-  <si>
-    <t>9d2f95e489ceddbf4243312786fc051c</t>
-  </si>
-  <si>
-    <t>75983dd64ff91a59ef57e3b07b0cdd27</t>
-  </si>
-  <si>
-    <t>22d7a20d64e9a710bd5002decbc7ab92</t>
-  </si>
-  <si>
-    <t>b0e5279ee4b3ca75dfdbc084b1a6acdc</t>
-  </si>
-  <si>
-    <t>ec06a4d916620dfeaafa04f0ba10ee7e</t>
-  </si>
-  <si>
-    <t>335c16de10f3c6ab274717d00364927c</t>
-  </si>
-  <si>
-    <t>7770f6e518cc9b085df2ea5ad1c54932</t>
-  </si>
-  <si>
-    <t>16c6e3500d9d9bd3de38ccb74c4ec8f4</t>
-  </si>
-  <si>
-    <t>067db59e642f8b47753f3ed304d3f352</t>
-  </si>
-  <si>
-    <t>464ef65c65984fbeee1a80742f1ce4ba</t>
-  </si>
-  <si>
-    <t>f6cc6923dfa81a5f77f65ac2682d83ab</t>
-  </si>
-  <si>
-    <t>895d030ee4458eef34d860175df80098</t>
-  </si>
-  <si>
-    <t>287cd2ba6e4696482554c794615aae39</t>
-  </si>
-  <si>
-    <t>387e7ed7737fa1cc098f4a5d2bbcaa0c</t>
-  </si>
-  <si>
-    <t>0ec676713ec1c6b31acc77f64d4b5398</t>
-  </si>
-  <si>
-    <t>e4ad17c76a402971882e7890e6f8b960</t>
-  </si>
-  <si>
-    <t>69f26998934f4b46eb143301515e4c27</t>
-  </si>
-  <si>
-    <t>35f5eee88e40abc0a5edfd61a36bc839</t>
-  </si>
-  <si>
-    <t>0233943885a016ad567da2009f12bf12</t>
-  </si>
-  <si>
-    <t>5e9ac4c4f4645da04f945d6357478f37</t>
-  </si>
-  <si>
-    <t>3670ee43dc6935180ded2f42a00a37fd</t>
-  </si>
-  <si>
-    <t>4b92aca60fa7305ae587de9098874107</t>
-  </si>
-  <si>
-    <t>8a6a6c5f2a18bb7d7e9eee697eef5ec9</t>
-  </si>
-  <si>
-    <t>beb2a42e080e245af46f17cd07644400</t>
-  </si>
-  <si>
-    <t>6959efec9c68cf1172a40a4db191948d</t>
-  </si>
-  <si>
-    <t>1350a094690f58fafac140ffbecd08cf</t>
-  </si>
-  <si>
-    <t>85548c47aca9dcbd6712f0a8442c954c</t>
-  </si>
-  <si>
-    <t>1b562ad2a8d24502d0fa02ae9986dcd2</t>
-  </si>
-  <si>
-    <t>ed0ed0d4228374fc5a3412c6ae702f18</t>
-  </si>
-  <si>
-    <t>dfce06b1ab799daef2999a3f7a54e66c</t>
-  </si>
-  <si>
-    <t>889457057abfb48eba9b7d37bc4719dd</t>
-  </si>
-  <si>
-    <t>197f95adc74e5d1ee9f60f5c1723295d</t>
-  </si>
-  <si>
-    <t>24a9f3dfd987963f89eac0f984e96512</t>
-  </si>
-  <si>
-    <t>88cb1f096567362f766916e764fd94f2</t>
-  </si>
-  <si>
-    <t>85a313e298ad1f4e28a2b248c8722dd1</t>
-  </si>
-  <si>
-    <t>f79adbe570bbcf13f1edac31d32ecb24</t>
-  </si>
-  <si>
-    <t>3b5d03807d0d0621de987d354f70647b</t>
-  </si>
-  <si>
-    <t>7d518978281dea44bc781ab11add19cc</t>
-  </si>
-  <si>
-    <t>6a710ea4f259419044c5fba4e7312cfb</t>
-  </si>
-  <si>
-    <t>5fdc7a2b4c6ffef4c16f9a6f7a547e86</t>
-  </si>
-  <si>
-    <t>bdbc2ce6b58232f8b2cd38367c4eb0f9</t>
-  </si>
-  <si>
-    <t>c87b0c2d47ec2ade935c1c8028cf69e8</t>
-  </si>
-  <si>
-    <t>51011dd14ecd94a97984578c579b062d</t>
-  </si>
-  <si>
-    <t>6691923c8f53ba70d278663a9bb3e198</t>
-  </si>
-  <si>
-    <t>8e55b193ba8ef346d013e8eda8f154b1</t>
-  </si>
-  <si>
-    <t>492791b818f954cc2c8cb64d06fa0075</t>
-  </si>
-  <si>
-    <t>6ba681bfb6d2d44dd0c534e07d6f0149</t>
-  </si>
-  <si>
-    <t>26a7bd1fa638362aef3ca8b16683b347</t>
+    <t>e632913b8d7f4aea2d311f087b0eb220</t>
+  </si>
+  <si>
+    <t>ed21f81d5d66130b4decb13147462201</t>
+  </si>
+  <si>
+    <t>f077baa5af7f692e7e192b6af89ee86a</t>
+  </si>
+  <si>
+    <t>125b0b6d24dd75c74b180005df0cbe15</t>
+  </si>
+  <si>
+    <t>def883d3d420a041f58125d18b7ade75</t>
+  </si>
+  <si>
+    <t>e6ea358366c150b9e0f80ba6ec7060b4</t>
+  </si>
+  <si>
+    <t>d7ee44f53f3828cc936c73f3690086ce</t>
+  </si>
+  <si>
+    <t>a7cc5dc136392dbad400510c48863791</t>
+  </si>
+  <si>
+    <t>d0dee0589c8737ec2f6048b08b2b9f27</t>
+  </si>
+  <si>
+    <t>e829e35ac7481feb91c8effe4feb9949</t>
+  </si>
+  <si>
+    <t>66dd60fbf9579e00829599be99e4e612</t>
+  </si>
+  <si>
+    <t>ebdb2cc84806456439e12fcec47f121e</t>
+  </si>
+  <si>
+    <t>954097849c87c889c95051c51d93c0db</t>
+  </si>
+  <si>
+    <t>68506212939aa0b2a718d52c0c87a7c0</t>
+  </si>
+  <si>
+    <t>e594f8d0f3ef3aeca7f8bf0696246f7c</t>
+  </si>
+  <si>
+    <t>b820a0eaa2c5ebfe9fdc9d6979e6d5f1</t>
+  </si>
+  <si>
+    <t>29db4fd9d19daeb033a372d2fee2f138</t>
+  </si>
+  <si>
+    <t>82ec219f87c8c64af79033cef2c7ad0f</t>
+  </si>
+  <si>
+    <t>87219f9033db548ec3e3c0c40a169abf</t>
+  </si>
+  <si>
+    <t>49638f8a40fdda685945c7546344a796</t>
+  </si>
+  <si>
+    <t>33497e5a32db90e49130163ef47548c1</t>
+  </si>
+  <si>
+    <t>88377659d16317d88daebd0b8107ad4c</t>
+  </si>
+  <si>
+    <t>fe9f13143212c79f372c062a6331398e</t>
+  </si>
+  <si>
+    <t>2a2bc2f11f62d2a53509644e876d7d91</t>
+  </si>
+  <si>
+    <t>e6a046b94f40a82e32de53b994b80864</t>
+  </si>
+  <si>
+    <t>f9687f7e0db9f6855d5e67b6aeb8826c</t>
+  </si>
+  <si>
+    <t>12ee17cfec0214ffc02800de4a24f2a1</t>
+  </si>
+  <si>
+    <t>87ff54070d4a466a676290296771212d</t>
+  </si>
+  <si>
+    <t>1167bb6ee18832cf27f41231cd86f1ca</t>
+  </si>
+  <si>
+    <t>7d011e2cbb678b75055cc1b555e53bcc</t>
+  </si>
+  <si>
+    <t>fbcdcf2fced71087e1e898d71148a481</t>
+  </si>
+  <si>
+    <t>84f5445bcc9b25f5f779143b79a04ee5</t>
+  </si>
+  <si>
+    <t>9646838b987f0fd06d18dab1818206a5</t>
+  </si>
+  <si>
+    <t>74e315e8ecd9587de2499598c918c258</t>
+  </si>
+  <si>
+    <t>0ac1df1c5b1d69b731b2f3fea911b5d6</t>
+  </si>
+  <si>
+    <t>d8b1758c2d84b1be94535b7ff9d1e39d</t>
+  </si>
+  <si>
+    <t>65083e5e41a89bb6d36f4c24e805da71</t>
+  </si>
+  <si>
+    <t>913cf8aaf6ed1935e29763d336691b66</t>
+  </si>
+  <si>
+    <t>ea593202116ee4bda2945d84b2fd9224</t>
+  </si>
+  <si>
+    <t>2e35bed4626da39dda908a908309fcab</t>
+  </si>
+  <si>
+    <t>6d8d39e569cd7818ed12e61c61aba68e</t>
+  </si>
+  <si>
+    <t>ea01203dd6d023c91bc19b6de59bd7af</t>
+  </si>
+  <si>
+    <t>28bc7daca3887f3ca7f20aa3c6c63e66</t>
+  </si>
+  <si>
+    <t>e780f82f788b492b4a3dc55f0432de3f</t>
+  </si>
+  <si>
+    <t>251dccb6699bc82a012c148ca7314439</t>
+  </si>
+  <si>
+    <t>98dc51d9b23012482d47df6fe969db2a</t>
+  </si>
+  <si>
+    <t>d00ffd2ac9a7c2211a463bb9fd4f3c2f</t>
+  </si>
+  <si>
+    <t>df91d71dcea9996f856529476df10bd3</t>
+  </si>
+  <si>
+    <t>b1255f925515510f5b01282716660dc6</t>
+  </si>
+  <si>
+    <t>ef7d8fad48c6405b96643da1360a34ee</t>
+  </si>
+  <si>
+    <t>81ecd1d78ea0dfd304467442038ca560</t>
+  </si>
+  <si>
+    <t>87c628468a3d8da5770ff1ba4b2bda7d</t>
+  </si>
+  <si>
+    <t>5582928e01f4f7efd1bf5d80c2e05fd1</t>
+  </si>
+  <si>
+    <t>6600be176cbc6429df7fd8e4b1e8e07a</t>
+  </si>
+  <si>
+    <t>caa20c11db1be1954619264945bae17c</t>
+  </si>
+  <si>
+    <t>4ec0badcd05d49330d86358dd7cc33bb</t>
+  </si>
+  <si>
+    <t>008f075035c35ea04229e67052ef6b9a</t>
+  </si>
+  <si>
+    <t>d3793dd462a16e84804800b605515b45</t>
+  </si>
+  <si>
+    <t>600f24da2707aa72cbe2e65945a2602e</t>
+  </si>
+  <si>
+    <t>77a459c337c2e9f69db50faddc4b7035</t>
+  </si>
+  <si>
+    <t>6c71581e87cd00e3688dd89e8b815767</t>
+  </si>
+  <si>
+    <t>fffcab7789b869adb46832e7510e698c</t>
+  </si>
+  <si>
+    <t>baef94a2e401783472563823a7df73b2</t>
+  </si>
+  <si>
+    <t>133b3c1430e39899cd8bbcf8518bec3d</t>
+  </si>
+  <si>
+    <t>625bfa4139b7fd0ed1fd693b2ff9358d</t>
+  </si>
+  <si>
+    <t>c2093d2153f20db328676a11a4cd6a16</t>
+  </si>
+  <si>
+    <t>61293d4ea7d7dc08f7efff752bd00be0</t>
+  </si>
+  <si>
+    <t>96f4db8875321f2e03921cc2bd78dbd5</t>
+  </si>
+  <si>
+    <t>98fb80cbf3a2db0e040a9b927f345d7a</t>
+  </si>
+  <si>
+    <t>306643899569ce0f8c204d7648c72db6</t>
+  </si>
+  <si>
+    <t>95c2208ac063f2eb5e5cce9bf0a5ead8</t>
+  </si>
+  <si>
+    <t>08216ca4b0d8a27d0b36b09a7e24a18f</t>
+  </si>
+  <si>
+    <t>150a109faa495421a4a466207ad4789d</t>
+  </si>
+  <si>
+    <t>f7fc7695b5201e9a5cbb3cf2d24b9ed9</t>
+  </si>
+  <si>
+    <t>7da5d1f16fb8b1a03d20ddfa9713d1a7</t>
+  </si>
+  <si>
+    <t>eae5ace3036c46346a584360d7c3b588</t>
+  </si>
+  <si>
+    <t>e8d770fa7d75177fc67e33d9f960c94b</t>
+  </si>
+  <si>
+    <t>1d059e896a8771d48ed475bac5a64038</t>
+  </si>
+  <si>
+    <t>c5c7474b369bdd89e6d3e12a8959fb26</t>
+  </si>
+  <si>
+    <t>080df65bd756fa7e457a4944cd5ed9d3</t>
+  </si>
+  <si>
+    <t>d91015c653100b5b2a3c6ee31b80eab2</t>
+  </si>
+  <si>
+    <t>a6a223e6d3e50756996514fa3248e18f</t>
+  </si>
+  <si>
+    <t>faa677c0154793050c7d5dfa77e24be8</t>
+  </si>
+  <si>
+    <t>631ec3c72f3b65b111d61321f8fab58d</t>
+  </si>
+  <si>
+    <t>9f6cf110b05559492524d80ad16e0e7d</t>
+  </si>
+  <si>
+    <t>396caf8dfbc2d0cdbc51f09c1d1eb47c</t>
+  </si>
+  <si>
+    <t>9f64c158384ab8139fd9c217a7cfc5fc</t>
+  </si>
+  <si>
+    <t>03c28cb1f3a0e0a8122e9e411a7cd555</t>
+  </si>
+  <si>
+    <t>84f01a7fad3877393c8a88842a3c73c2</t>
+  </si>
+  <si>
+    <t>31deb70841a1487d740f9b3b4d17c046</t>
+  </si>
+  <si>
+    <t>89cfdea8602f0c6dd9384a534b03efce</t>
   </si>
 </sst>
 </file>
@@ -1304,7 +1304,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1327,6 +1327,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1668,14 +1669,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P28" sqref="P28"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="27" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1" max="15" width="25.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="35.42578125" style="1" customWidth="1"/>
+    <col min="17" max="27" width="25.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="2" customFormat="1" ht="126" x14ac:dyDescent="0.25">
@@ -1858,7 +1861,7 @@
         <v>74</v>
       </c>
       <c r="I5">
-        <v>11931213</v>
+        <v>12958024</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>107</v>
@@ -1867,7 +1870,7 @@
         <v>203</v>
       </c>
       <c r="P5" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="R5" s="5" t="s">
         <v>78</v>
@@ -1888,7 +1891,7 @@
         <v>74</v>
       </c>
       <c r="I6">
-        <v>11931212</v>
+        <v>12958021</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>107</v>
@@ -1897,7 +1900,7 @@
         <v>204</v>
       </c>
       <c r="P6" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="R6" s="5" t="s">
         <v>78</v>
@@ -1918,7 +1921,7 @@
         <v>74</v>
       </c>
       <c r="I7">
-        <v>11657552</v>
+        <v>12685331</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>107</v>
@@ -1927,7 +1930,7 @@
         <v>205</v>
       </c>
       <c r="P7" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="R7" s="5" t="s">
         <v>78</v>
@@ -1948,7 +1951,7 @@
         <v>74</v>
       </c>
       <c r="I8">
-        <v>11659544</v>
+        <v>12687024</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>107</v>
@@ -1957,7 +1960,7 @@
         <v>206</v>
       </c>
       <c r="P8" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="R8" s="5" t="s">
         <v>78</v>
@@ -1978,7 +1981,7 @@
         <v>74</v>
       </c>
       <c r="I9">
-        <v>11931569</v>
+        <v>12958290</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>107</v>
@@ -1987,7 +1990,7 @@
         <v>207</v>
       </c>
       <c r="P9" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="R9" s="5" t="s">
         <v>78</v>
@@ -2008,7 +2011,7 @@
         <v>74</v>
       </c>
       <c r="I10">
-        <v>11931580</v>
+        <v>12958301</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>107</v>
@@ -2017,7 +2020,7 @@
         <v>208</v>
       </c>
       <c r="P10" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="R10" s="5" t="s">
         <v>78</v>
@@ -2038,7 +2041,7 @@
         <v>74</v>
       </c>
       <c r="I11">
-        <v>11930390</v>
+        <v>12957206</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>107</v>
@@ -2047,7 +2050,7 @@
         <v>209</v>
       </c>
       <c r="P11" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="R11" s="5" t="s">
         <v>78</v>
@@ -2068,7 +2071,7 @@
         <v>74</v>
       </c>
       <c r="I12">
-        <v>11930591</v>
+        <v>12957400</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>107</v>
@@ -2077,7 +2080,7 @@
         <v>210</v>
       </c>
       <c r="P12" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="R12" s="5" t="s">
         <v>78</v>
@@ -2098,7 +2101,7 @@
         <v>74</v>
       </c>
       <c r="I13">
-        <v>11931215</v>
+        <v>12958026</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>107</v>
@@ -2107,7 +2110,7 @@
         <v>211</v>
       </c>
       <c r="P13" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="R13" s="5" t="s">
         <v>78</v>
@@ -2128,7 +2131,7 @@
         <v>74</v>
       </c>
       <c r="I14">
-        <v>11931169</v>
+        <v>12957980</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>107</v>
@@ -2137,7 +2140,7 @@
         <v>212</v>
       </c>
       <c r="P14" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="R14" s="5" t="s">
         <v>78</v>
@@ -2158,7 +2161,7 @@
         <v>74</v>
       </c>
       <c r="I15">
-        <v>11931211</v>
+        <v>12958021</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>107</v>
@@ -2167,7 +2170,7 @@
         <v>213</v>
       </c>
       <c r="P15" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="R15" s="5" t="s">
         <v>78</v>
@@ -2188,7 +2191,7 @@
         <v>74</v>
       </c>
       <c r="I16">
-        <v>11930666</v>
+        <v>12957480</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>107</v>
@@ -2197,7 +2200,7 @@
         <v>214</v>
       </c>
       <c r="P16" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="R16" s="5" t="s">
         <v>78</v>
@@ -2218,7 +2221,7 @@
         <v>74</v>
       </c>
       <c r="I17">
-        <v>11931541</v>
+        <v>12958254</v>
       </c>
       <c r="M17" s="1" t="s">
         <v>107</v>
@@ -2227,7 +2230,7 @@
         <v>215</v>
       </c>
       <c r="P17" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="R17" s="5" t="s">
         <v>78</v>
@@ -2248,7 +2251,7 @@
         <v>74</v>
       </c>
       <c r="I18">
-        <v>11931151</v>
+        <v>12957958</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>107</v>
@@ -2257,7 +2260,7 @@
         <v>216</v>
       </c>
       <c r="P18" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="R18" s="5" t="s">
         <v>78</v>
@@ -2278,7 +2281,7 @@
         <v>74</v>
       </c>
       <c r="I19">
-        <v>11931212</v>
+        <v>12958023</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>107</v>
@@ -2287,7 +2290,7 @@
         <v>217</v>
       </c>
       <c r="P19" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="R19" s="5" t="s">
         <v>78</v>
@@ -2308,7 +2311,7 @@
         <v>74</v>
       </c>
       <c r="I20">
-        <v>11931188</v>
+        <v>12957995</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>107</v>
@@ -2317,7 +2320,7 @@
         <v>218</v>
       </c>
       <c r="P20" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="R20" s="5" t="s">
         <v>78</v>
@@ -2338,7 +2341,7 @@
         <v>74</v>
       </c>
       <c r="I21">
-        <v>11930734</v>
+        <v>12957572</v>
       </c>
       <c r="M21" s="1" t="s">
         <v>107</v>
@@ -2347,7 +2350,7 @@
         <v>219</v>
       </c>
       <c r="P21" t="s">
-        <v>297</v>
+        <v>309</v>
       </c>
       <c r="R21" s="5" t="s">
         <v>78</v>
@@ -2368,7 +2371,7 @@
         <v>74</v>
       </c>
       <c r="I22">
-        <v>11930589</v>
+        <v>12957401</v>
       </c>
       <c r="M22" s="1" t="s">
         <v>107</v>
@@ -2377,7 +2380,7 @@
         <v>220</v>
       </c>
       <c r="P22" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="R22" s="5" t="s">
         <v>78</v>
@@ -2398,7 +2401,7 @@
         <v>74</v>
       </c>
       <c r="I23">
-        <v>11930521</v>
+        <v>12957362</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>107</v>
@@ -2407,7 +2410,7 @@
         <v>221</v>
       </c>
       <c r="P23" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="R23" s="5" t="s">
         <v>78</v>
@@ -2428,7 +2431,7 @@
         <v>74</v>
       </c>
       <c r="I24">
-        <v>11931202</v>
+        <v>12958010</v>
       </c>
       <c r="M24" s="1" t="s">
         <v>107</v>
@@ -2437,7 +2440,7 @@
         <v>222</v>
       </c>
       <c r="P24" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="R24" s="5" t="s">
         <v>78</v>
@@ -2458,7 +2461,7 @@
         <v>74</v>
       </c>
       <c r="I25">
-        <v>11931108</v>
+        <v>12957856</v>
       </c>
       <c r="M25" s="1" t="s">
         <v>107</v>
@@ -2467,7 +2470,7 @@
         <v>223</v>
       </c>
       <c r="P25" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="R25" s="5" t="s">
         <v>78</v>
@@ -2488,7 +2491,7 @@
         <v>74</v>
       </c>
       <c r="I26">
-        <v>11931215</v>
+        <v>12958026</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>107</v>
@@ -2497,7 +2500,7 @@
         <v>224</v>
       </c>
       <c r="P26" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="R26" s="5" t="s">
         <v>78</v>
@@ -2518,7 +2521,7 @@
         <v>74</v>
       </c>
       <c r="I27">
-        <v>11931575</v>
+        <v>12958296</v>
       </c>
       <c r="M27" s="1" t="s">
         <v>107</v>
@@ -2527,7 +2530,7 @@
         <v>225</v>
       </c>
       <c r="P27" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="R27" s="5" t="s">
         <v>78</v>
@@ -2548,7 +2551,7 @@
         <v>74</v>
       </c>
       <c r="I28">
-        <v>11931216</v>
+        <v>12958024</v>
       </c>
       <c r="M28" s="1" t="s">
         <v>107</v>
@@ -2557,7 +2560,7 @@
         <v>226</v>
       </c>
       <c r="P28" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="R28" s="5" t="s">
         <v>78</v>
@@ -2578,7 +2581,7 @@
         <v>74</v>
       </c>
       <c r="I29">
-        <v>11931207</v>
+        <v>12958018</v>
       </c>
       <c r="M29" s="1" t="s">
         <v>107</v>
@@ -2587,7 +2590,7 @@
         <v>227</v>
       </c>
       <c r="P29" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="R29" s="5" t="s">
         <v>78</v>
@@ -2608,7 +2611,7 @@
         <v>74</v>
       </c>
       <c r="I30">
-        <v>11931558</v>
+        <v>12958279</v>
       </c>
       <c r="M30" s="1" t="s">
         <v>107</v>
@@ -2617,7 +2620,7 @@
         <v>228</v>
       </c>
       <c r="P30" t="s">
-        <v>293</v>
+        <v>318</v>
       </c>
       <c r="R30" s="5" t="s">
         <v>78</v>
@@ -2638,7 +2641,7 @@
         <v>74</v>
       </c>
       <c r="I31">
-        <v>11930637</v>
+        <v>12957464</v>
       </c>
       <c r="M31" s="1" t="s">
         <v>107</v>
@@ -2647,7 +2650,7 @@
         <v>229</v>
       </c>
       <c r="P31" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="R31" s="5" t="s">
         <v>78</v>
@@ -2668,7 +2671,7 @@
         <v>74</v>
       </c>
       <c r="I32">
-        <v>11930750</v>
+        <v>12957591</v>
       </c>
       <c r="M32" s="1" t="s">
         <v>107</v>
@@ -2677,7 +2680,7 @@
         <v>230</v>
       </c>
       <c r="P32" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="R32" s="5" t="s">
         <v>78</v>
@@ -2698,7 +2701,7 @@
         <v>74</v>
       </c>
       <c r="I33">
-        <v>11931492</v>
+        <v>12958213</v>
       </c>
       <c r="M33" s="1" t="s">
         <v>107</v>
@@ -2707,7 +2710,7 @@
         <v>231</v>
       </c>
       <c r="P33" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="R33" s="5" t="s">
         <v>78</v>
@@ -2728,7 +2731,7 @@
         <v>74</v>
       </c>
       <c r="I34">
-        <v>11931575</v>
+        <v>12958296</v>
       </c>
       <c r="M34" s="1" t="s">
         <v>107</v>
@@ -2737,7 +2740,7 @@
         <v>232</v>
       </c>
       <c r="P34" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="R34" s="5" t="s">
         <v>78</v>
@@ -2758,7 +2761,7 @@
         <v>74</v>
       </c>
       <c r="I35">
-        <v>11931258</v>
+        <v>12957981</v>
       </c>
       <c r="M35" s="1" t="s">
         <v>107</v>
@@ -2767,7 +2770,7 @@
         <v>233</v>
       </c>
       <c r="P35" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="R35" s="5" t="s">
         <v>78</v>
@@ -2788,7 +2791,7 @@
         <v>74</v>
       </c>
       <c r="I36">
-        <v>11931081</v>
+        <v>12957890</v>
       </c>
       <c r="M36" s="1" t="s">
         <v>107</v>
@@ -2797,7 +2800,7 @@
         <v>234</v>
       </c>
       <c r="P36" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="R36" s="5" t="s">
         <v>78</v>
@@ -2818,7 +2821,7 @@
         <v>74</v>
       </c>
       <c r="I37">
-        <v>11658151</v>
+        <v>12685639</v>
       </c>
       <c r="M37" s="1" t="s">
         <v>107</v>
@@ -2827,7 +2830,7 @@
         <v>235</v>
       </c>
       <c r="P37" t="s">
-        <v>294</v>
+        <v>325</v>
       </c>
       <c r="R37" s="5" t="s">
         <v>78</v>
@@ -2848,7 +2851,7 @@
         <v>74</v>
       </c>
       <c r="I38">
-        <v>11930461</v>
+        <v>12957312</v>
       </c>
       <c r="M38" s="1" t="s">
         <v>107</v>
@@ -2856,8 +2859,8 @@
       <c r="O38" t="s">
         <v>236</v>
       </c>
-      <c r="P38" t="s">
-        <v>329</v>
+      <c r="P38" s="10" t="s">
+        <v>326</v>
       </c>
       <c r="R38" s="5" t="s">
         <v>78</v>
@@ -2878,7 +2881,7 @@
         <v>74</v>
       </c>
       <c r="I39">
-        <v>11931206</v>
+        <v>12958018</v>
       </c>
       <c r="M39" s="1" t="s">
         <v>107</v>
@@ -2887,7 +2890,7 @@
         <v>237</v>
       </c>
       <c r="P39" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="R39" s="5" t="s">
         <v>78</v>
@@ -2908,7 +2911,7 @@
         <v>74</v>
       </c>
       <c r="I40">
-        <v>11930655</v>
+        <v>12957466</v>
       </c>
       <c r="M40" s="1" t="s">
         <v>107</v>
@@ -2917,7 +2920,7 @@
         <v>238</v>
       </c>
       <c r="P40" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="R40" s="5" t="s">
         <v>78</v>
@@ -2938,7 +2941,7 @@
         <v>74</v>
       </c>
       <c r="I41">
-        <v>11659526</v>
+        <v>12687006</v>
       </c>
       <c r="M41" s="1" t="s">
         <v>107</v>
@@ -2947,7 +2950,7 @@
         <v>239</v>
       </c>
       <c r="P41" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="R41" s="5" t="s">
         <v>78</v>
@@ -2968,7 +2971,7 @@
         <v>74</v>
       </c>
       <c r="I42">
-        <v>11931462</v>
+        <v>12958183</v>
       </c>
       <c r="M42" s="1" t="s">
         <v>107</v>
@@ -2977,7 +2980,7 @@
         <v>240</v>
       </c>
       <c r="P42" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="R42" s="5" t="s">
         <v>78</v>
@@ -2998,7 +3001,7 @@
         <v>74</v>
       </c>
       <c r="I43">
-        <v>11659548</v>
+        <v>12687028</v>
       </c>
       <c r="M43" s="1" t="s">
         <v>107</v>
@@ -3007,7 +3010,7 @@
         <v>241</v>
       </c>
       <c r="P43" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="R43" s="5" t="s">
         <v>78</v>
@@ -3028,7 +3031,7 @@
         <v>74</v>
       </c>
       <c r="I44">
-        <v>11930636</v>
+        <v>12957474</v>
       </c>
       <c r="M44" s="1" t="s">
         <v>107</v>
@@ -3037,7 +3040,7 @@
         <v>242</v>
       </c>
       <c r="P44" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="R44" s="5" t="s">
         <v>78</v>
@@ -3058,7 +3061,7 @@
         <v>74</v>
       </c>
       <c r="I45">
-        <v>11931205</v>
+        <v>12958012</v>
       </c>
       <c r="M45" s="1" t="s">
         <v>107</v>
@@ -3067,7 +3070,7 @@
         <v>243</v>
       </c>
       <c r="P45" t="s">
-        <v>298</v>
+        <v>333</v>
       </c>
       <c r="R45" s="5" t="s">
         <v>78</v>
@@ -3088,7 +3091,7 @@
         <v>74</v>
       </c>
       <c r="I46">
-        <v>11659445</v>
+        <v>12686926</v>
       </c>
       <c r="M46" s="1" t="s">
         <v>107</v>
@@ -3097,7 +3100,7 @@
         <v>244</v>
       </c>
       <c r="P46" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="R46" s="5" t="s">
         <v>78</v>
@@ -3118,7 +3121,7 @@
         <v>74</v>
       </c>
       <c r="I47">
-        <v>11659098</v>
+        <v>12686578</v>
       </c>
       <c r="M47" s="1" t="s">
         <v>107</v>
@@ -3127,7 +3130,7 @@
         <v>245</v>
       </c>
       <c r="P47" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="R47" s="5" t="s">
         <v>78</v>
@@ -3148,7 +3151,7 @@
         <v>74</v>
       </c>
       <c r="I48">
-        <v>11658304</v>
+        <v>12686079</v>
       </c>
       <c r="M48" s="1" t="s">
         <v>107</v>
@@ -3157,7 +3160,7 @@
         <v>246</v>
       </c>
       <c r="P48" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="R48" s="5" t="s">
         <v>78</v>
@@ -3178,7 +3181,7 @@
         <v>74</v>
       </c>
       <c r="I49">
-        <v>11659545</v>
+        <v>12687025</v>
       </c>
       <c r="M49" s="1" t="s">
         <v>107</v>
@@ -3187,7 +3190,7 @@
         <v>247</v>
       </c>
       <c r="P49" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="R49" s="5" t="s">
         <v>78</v>
@@ -3208,7 +3211,7 @@
         <v>74</v>
       </c>
       <c r="I50">
-        <v>11931580</v>
+        <v>12958301</v>
       </c>
       <c r="M50" s="1" t="s">
         <v>107</v>
@@ -3217,7 +3220,7 @@
         <v>248</v>
       </c>
       <c r="P50" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="R50" s="5" t="s">
         <v>78</v>
@@ -3238,7 +3241,7 @@
         <v>74</v>
       </c>
       <c r="I51">
-        <v>11931560</v>
+        <v>12958280</v>
       </c>
       <c r="M51" s="1" t="s">
         <v>107</v>
@@ -3247,7 +3250,7 @@
         <v>249</v>
       </c>
       <c r="P51" t="s">
-        <v>295</v>
+        <v>339</v>
       </c>
       <c r="R51" s="5" t="s">
         <v>78</v>
@@ -3268,7 +3271,7 @@
         <v>74</v>
       </c>
       <c r="I52">
-        <v>11658438</v>
+        <v>12685920</v>
       </c>
       <c r="M52" s="1" t="s">
         <v>107</v>
@@ -3277,7 +3280,7 @@
         <v>250</v>
       </c>
       <c r="P52" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="R52" s="5" t="s">
         <v>78</v>
@@ -3298,7 +3301,7 @@
         <v>74</v>
       </c>
       <c r="I53">
-        <v>11657814</v>
+        <v>12685297</v>
       </c>
       <c r="M53" s="1" t="s">
         <v>107</v>
@@ -3307,7 +3310,7 @@
         <v>251</v>
       </c>
       <c r="P53" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="R53" s="5" t="s">
         <v>78</v>
@@ -3328,7 +3331,7 @@
         <v>74</v>
       </c>
       <c r="I54">
-        <v>11658083</v>
+        <v>12685860</v>
       </c>
       <c r="M54" s="1" t="s">
         <v>107</v>
@@ -3337,7 +3340,7 @@
         <v>252</v>
       </c>
       <c r="P54" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="R54" s="5" t="s">
         <v>78</v>
@@ -3358,7 +3361,7 @@
         <v>74</v>
       </c>
       <c r="I55">
-        <v>11658881</v>
+        <v>12686362</v>
       </c>
       <c r="M55" s="1" t="s">
         <v>107</v>
@@ -3367,7 +3370,7 @@
         <v>253</v>
       </c>
       <c r="P55" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="R55" s="5" t="s">
         <v>78</v>
@@ -3388,7 +3391,7 @@
         <v>74</v>
       </c>
       <c r="I56">
-        <v>11659538</v>
+        <v>12687018</v>
       </c>
       <c r="M56" s="1" t="s">
         <v>107</v>
@@ -3397,7 +3400,7 @@
         <v>254</v>
       </c>
       <c r="P56" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="R56" s="5" t="s">
         <v>78</v>
@@ -3418,7 +3421,7 @@
         <v>74</v>
       </c>
       <c r="I57">
-        <v>11658703</v>
+        <v>12686477</v>
       </c>
       <c r="M57" s="1" t="s">
         <v>107</v>
@@ -3427,7 +3430,7 @@
         <v>255</v>
       </c>
       <c r="P57" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="R57" s="5" t="s">
         <v>78</v>
@@ -3448,7 +3451,7 @@
         <v>74</v>
       </c>
       <c r="I58">
-        <v>11659503</v>
+        <v>12686983</v>
       </c>
       <c r="M58" s="1" t="s">
         <v>107</v>
@@ -3457,7 +3460,7 @@
         <v>256</v>
       </c>
       <c r="P58" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="R58" s="5" t="s">
         <v>78</v>
@@ -3478,7 +3481,7 @@
         <v>74</v>
       </c>
       <c r="I59">
-        <v>11659547</v>
+        <v>12687027</v>
       </c>
       <c r="M59" s="1" t="s">
         <v>107</v>
@@ -3487,7 +3490,7 @@
         <v>257</v>
       </c>
       <c r="P59" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="R59" s="5" t="s">
         <v>78</v>
@@ -3508,7 +3511,7 @@
         <v>74</v>
       </c>
       <c r="I60">
-        <v>11659520</v>
+        <v>12687001</v>
       </c>
       <c r="M60" s="1" t="s">
         <v>107</v>
@@ -3517,7 +3520,7 @@
         <v>258</v>
       </c>
       <c r="P60" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="R60" s="5" t="s">
         <v>78</v>
@@ -3538,7 +3541,7 @@
         <v>74</v>
       </c>
       <c r="I61">
-        <v>11659133</v>
+        <v>12686613</v>
       </c>
       <c r="M61" s="1" t="s">
         <v>107</v>
@@ -3547,7 +3550,7 @@
         <v>259</v>
       </c>
       <c r="P61" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="R61" s="5" t="s">
         <v>78</v>
@@ -3568,7 +3571,7 @@
         <v>74</v>
       </c>
       <c r="I62">
-        <v>11931047</v>
+        <v>12957771</v>
       </c>
       <c r="M62" s="1" t="s">
         <v>107</v>
@@ -3577,7 +3580,7 @@
         <v>260</v>
       </c>
       <c r="P62" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="R62" s="5" t="s">
         <v>78</v>
@@ -3598,7 +3601,7 @@
         <v>74</v>
       </c>
       <c r="I63">
-        <v>11931218</v>
+        <v>12958029</v>
       </c>
       <c r="M63" s="1" t="s">
         <v>107</v>
@@ -3607,7 +3610,7 @@
         <v>261</v>
       </c>
       <c r="P63" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="R63" s="5" t="s">
         <v>78</v>
@@ -3628,7 +3631,7 @@
         <v>74</v>
       </c>
       <c r="I64">
-        <v>11931579</v>
+        <v>12958300</v>
       </c>
       <c r="M64" s="1" t="s">
         <v>107</v>
@@ -3637,7 +3640,7 @@
         <v>262</v>
       </c>
       <c r="P64" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="R64" s="5" t="s">
         <v>78</v>
@@ -3658,7 +3661,7 @@
         <v>74</v>
       </c>
       <c r="I65">
-        <v>11931192</v>
+        <v>12958007</v>
       </c>
       <c r="M65" s="1" t="s">
         <v>107</v>
@@ -3667,7 +3670,7 @@
         <v>263</v>
       </c>
       <c r="P65" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="R65" s="5" t="s">
         <v>78</v>
@@ -3688,7 +3691,7 @@
         <v>74</v>
       </c>
       <c r="I66">
-        <v>11659528</v>
+        <v>12687008</v>
       </c>
       <c r="M66" s="1" t="s">
         <v>107</v>
@@ -3697,7 +3700,7 @@
         <v>264</v>
       </c>
       <c r="P66" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="R66" s="5" t="s">
         <v>78</v>
@@ -3718,7 +3721,7 @@
         <v>74</v>
       </c>
       <c r="I67">
-        <v>11658246</v>
+        <v>12686022</v>
       </c>
       <c r="M67" s="1" t="s">
         <v>107</v>
@@ -3727,7 +3730,7 @@
         <v>110</v>
       </c>
       <c r="P67" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="R67" s="5" t="s">
         <v>78</v>
@@ -3748,7 +3751,7 @@
         <v>74</v>
       </c>
       <c r="I68">
-        <v>11929870</v>
+        <v>12956740</v>
       </c>
       <c r="M68" s="1" t="s">
         <v>107</v>
@@ -3757,7 +3760,7 @@
         <v>265</v>
       </c>
       <c r="P68" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="R68" s="5" t="s">
         <v>78</v>
@@ -3778,7 +3781,7 @@
         <v>74</v>
       </c>
       <c r="I69">
-        <v>11931210</v>
+        <v>12958020</v>
       </c>
       <c r="M69" s="1" t="s">
         <v>107</v>
@@ -3787,7 +3790,7 @@
         <v>266</v>
       </c>
       <c r="P69" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="R69" s="5" t="s">
         <v>78</v>
@@ -3808,7 +3811,7 @@
         <v>74</v>
       </c>
       <c r="I70">
-        <v>11657437</v>
+        <v>12685212</v>
       </c>
       <c r="M70" s="1" t="s">
         <v>107</v>
@@ -3817,7 +3820,7 @@
         <v>267</v>
       </c>
       <c r="P70" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="R70" s="5" t="s">
         <v>78</v>
@@ -3838,7 +3841,7 @@
         <v>74</v>
       </c>
       <c r="I71">
-        <v>11931205</v>
+        <v>12958013</v>
       </c>
       <c r="M71" s="1" t="s">
         <v>107</v>
@@ -3847,7 +3850,7 @@
         <v>268</v>
       </c>
       <c r="P71" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="R71" s="5" t="s">
         <v>78</v>
@@ -3868,7 +3871,7 @@
         <v>74</v>
       </c>
       <c r="I72">
-        <v>11931455</v>
+        <v>12958177</v>
       </c>
       <c r="M72" s="1" t="s">
         <v>107</v>
@@ -3877,7 +3880,7 @@
         <v>269</v>
       </c>
       <c r="P72" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="R72" s="5" t="s">
         <v>78</v>
@@ -3898,7 +3901,7 @@
         <v>74</v>
       </c>
       <c r="I73">
-        <v>11931571</v>
+        <v>12958289</v>
       </c>
       <c r="M73" s="1" t="s">
         <v>107</v>
@@ -3907,7 +3910,7 @@
         <v>270</v>
       </c>
       <c r="P73" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="R73" s="5" t="s">
         <v>78</v>
@@ -3928,7 +3931,7 @@
         <v>74</v>
       </c>
       <c r="I74">
-        <v>11931561</v>
+        <v>12958280</v>
       </c>
       <c r="M74" s="1" t="s">
         <v>107</v>
@@ -3937,7 +3940,7 @@
         <v>271</v>
       </c>
       <c r="P74" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="R74" s="5" t="s">
         <v>78</v>
@@ -3958,7 +3961,7 @@
         <v>74</v>
       </c>
       <c r="I75">
-        <v>11658964</v>
+        <v>12686445</v>
       </c>
       <c r="M75" s="1" t="s">
         <v>107</v>
@@ -3967,7 +3970,7 @@
         <v>272</v>
       </c>
       <c r="P75" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R75" s="5" t="s">
         <v>78</v>
@@ -3988,7 +3991,7 @@
         <v>74</v>
       </c>
       <c r="I76">
-        <v>11931561</v>
+        <v>12958282</v>
       </c>
       <c r="M76" s="1" t="s">
         <v>107</v>
@@ -3997,7 +4000,7 @@
         <v>273</v>
       </c>
       <c r="P76" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="R76" s="5" t="s">
         <v>78</v>
@@ -4018,7 +4021,7 @@
         <v>74</v>
       </c>
       <c r="I77">
-        <v>11930465</v>
+        <v>12957309</v>
       </c>
       <c r="M77" s="1" t="s">
         <v>107</v>
@@ -4027,7 +4030,7 @@
         <v>274</v>
       </c>
       <c r="P77" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="R77" s="5" t="s">
         <v>78</v>
@@ -4048,7 +4051,7 @@
         <v>74</v>
       </c>
       <c r="I78">
-        <v>11931209</v>
+        <v>12958020</v>
       </c>
       <c r="M78" s="1" t="s">
         <v>107</v>
@@ -4057,7 +4060,7 @@
         <v>275</v>
       </c>
       <c r="P78" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="R78" s="5" t="s">
         <v>78</v>
@@ -4078,7 +4081,7 @@
         <v>74</v>
       </c>
       <c r="I79">
-        <v>11931212</v>
+        <v>12958024</v>
       </c>
       <c r="M79" s="1" t="s">
         <v>107</v>
@@ -4087,7 +4090,7 @@
         <v>276</v>
       </c>
       <c r="P79" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="R79" s="5" t="s">
         <v>78</v>
@@ -4108,7 +4111,7 @@
         <v>74</v>
       </c>
       <c r="I80">
-        <v>11931210</v>
+        <v>12958021</v>
       </c>
       <c r="M80" s="1" t="s">
         <v>107</v>
@@ -4117,7 +4120,7 @@
         <v>277</v>
       </c>
       <c r="P80" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="R80" s="5" t="s">
         <v>78</v>
@@ -4138,7 +4141,7 @@
         <v>74</v>
       </c>
       <c r="I81">
-        <v>11931211</v>
+        <v>12958022</v>
       </c>
       <c r="M81" s="1" t="s">
         <v>107</v>
@@ -4147,7 +4150,7 @@
         <v>278</v>
       </c>
       <c r="P81" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="R81" s="5" t="s">
         <v>78</v>
@@ -4168,7 +4171,7 @@
         <v>74</v>
       </c>
       <c r="I82">
-        <v>11930323</v>
+        <v>12957168</v>
       </c>
       <c r="M82" s="1" t="s">
         <v>107</v>
@@ -4177,7 +4180,7 @@
         <v>279</v>
       </c>
       <c r="P82" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="R82" s="5" t="s">
         <v>78</v>
@@ -4198,7 +4201,7 @@
         <v>74</v>
       </c>
       <c r="I83">
-        <v>11659547</v>
+        <v>12687026</v>
       </c>
       <c r="M83" s="1" t="s">
         <v>107</v>
@@ -4207,7 +4210,7 @@
         <v>280</v>
       </c>
       <c r="P83" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="R83" s="5" t="s">
         <v>78</v>
@@ -4228,7 +4231,7 @@
         <v>74</v>
       </c>
       <c r="I84">
-        <v>11931220</v>
+        <v>12958031</v>
       </c>
       <c r="M84" s="1" t="s">
         <v>107</v>
@@ -4237,7 +4240,7 @@
         <v>281</v>
       </c>
       <c r="P84" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="R84" s="5" t="s">
         <v>78</v>
@@ -4258,7 +4261,7 @@
         <v>74</v>
       </c>
       <c r="I85">
-        <v>11930773</v>
+        <v>12957586</v>
       </c>
       <c r="M85" s="1" t="s">
         <v>107</v>
@@ -4267,7 +4270,7 @@
         <v>282</v>
       </c>
       <c r="P85" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="R85" s="5" t="s">
         <v>78</v>
@@ -4288,7 +4291,7 @@
         <v>74</v>
       </c>
       <c r="I86">
-        <v>11658710</v>
+        <v>12686484</v>
       </c>
       <c r="M86" s="1" t="s">
         <v>107</v>
@@ -4297,7 +4300,7 @@
         <v>283</v>
       </c>
       <c r="P86" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="R86" s="5" t="s">
         <v>78</v>
@@ -4318,7 +4321,7 @@
         <v>74</v>
       </c>
       <c r="I87">
-        <v>11659042</v>
+        <v>12686475</v>
       </c>
       <c r="M87" s="1" t="s">
         <v>107</v>
@@ -4327,7 +4330,7 @@
         <v>284</v>
       </c>
       <c r="P87" t="s">
-        <v>299</v>
+        <v>375</v>
       </c>
       <c r="R87" s="5" t="s">
         <v>78</v>
@@ -4348,7 +4351,7 @@
         <v>74</v>
       </c>
       <c r="I88">
-        <v>11658233</v>
+        <v>12686010</v>
       </c>
       <c r="M88" s="1" t="s">
         <v>107</v>
@@ -4378,7 +4381,7 @@
         <v>74</v>
       </c>
       <c r="I89">
-        <v>11659544</v>
+        <v>12687022</v>
       </c>
       <c r="M89" s="1" t="s">
         <v>107</v>
@@ -4408,7 +4411,7 @@
         <v>74</v>
       </c>
       <c r="I90">
-        <v>11930731</v>
+        <v>12957573</v>
       </c>
       <c r="M90" s="1" t="s">
         <v>107</v>
@@ -4438,7 +4441,7 @@
         <v>74</v>
       </c>
       <c r="I91">
-        <v>11931211</v>
+        <v>12958022</v>
       </c>
       <c r="M91" s="1" t="s">
         <v>107</v>
@@ -4468,7 +4471,7 @@
         <v>74</v>
       </c>
       <c r="I92">
-        <v>11659531</v>
+        <v>12687011</v>
       </c>
       <c r="M92" s="1" t="s">
         <v>107</v>
@@ -4498,7 +4501,7 @@
         <v>74</v>
       </c>
       <c r="I93">
-        <v>11931210</v>
+        <v>12958021</v>
       </c>
       <c r="M93" s="1" t="s">
         <v>107</v>
@@ -4528,7 +4531,7 @@
         <v>74</v>
       </c>
       <c r="I94">
-        <v>11930645</v>
+        <v>12957460</v>
       </c>
       <c r="M94" s="1" t="s">
         <v>107</v>
@@ -4558,7 +4561,7 @@
         <v>74</v>
       </c>
       <c r="I95">
-        <v>11931560</v>
+        <v>12958279</v>
       </c>
       <c r="M95" s="1" t="s">
         <v>107</v>
@@ -4619,9 +4622,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M95"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>